<commit_message>
Add cascade series plot
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_sir_dynamic.xlsx
+++ b/tests/databooks/databook_sir_dynamic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F60575-838F-4FC6-812C-5D19EA8C4738}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954ED601-130C-486F-9381-C00D885F61BA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -699,7 +699,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,13 +796,13 @@
         <v>6</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F5" s="2">
-        <v>60</v>
+        <v>260</v>
       </c>
       <c r="G5" s="2">
-        <v>80</v>
+        <v>280</v>
       </c>
       <c r="H5" s="2">
         <v>300</v>
@@ -848,13 +848,13 @@
         <v>1000</v>
       </c>
       <c r="F8" s="2">
-        <v>1000</v>
+        <v>990</v>
       </c>
       <c r="G8" s="2">
-        <v>1000</v>
+        <v>985</v>
       </c>
       <c r="H8" s="2">
-        <v>950</v>
+        <v>980</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -943,16 +943,16 @@
         <v>6</v>
       </c>
       <c r="E14" s="2">
-        <v>0</v>
+        <v>310</v>
       </c>
       <c r="F14" s="2">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="G14" s="2">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="H14" s="2">
-        <v>373</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>